<commit_message>
whole dry weights adjusted for early F1s
</commit_message>
<xml_diff>
--- a/RAnalysis/Data/Survival_Size/TDW_AFDW_Condition_master.xlsx
+++ b/RAnalysis/Data/Survival_Size/TDW_AFDW_Condition_master.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4704" yWindow="0" windowWidth="21864" windowHeight="9780"/>
+    <workbookView xWindow="5880" yWindow="0" windowWidth="21864" windowHeight="9780"/>
   </bookViews>
   <sheets>
     <sheet name="TDW_AFDW_Condition_master" sheetId="1" r:id="rId1"/>
@@ -1037,9 +1037,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z903"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J76" sqref="J76"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U17" sqref="U17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1088,7 +1088,7 @@
       <c r="K1" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="M1" s="1" t="s">
@@ -9219,13 +9219,14 @@
         <v>128</v>
       </c>
       <c r="S101" s="3">
-        <v>32.828000000000003</v>
+        <v>3.2828000000000003E-2</v>
       </c>
       <c r="T101" s="3">
-        <v>34.593000000000004</v>
+        <v>3.4593000000000006E-2</v>
       </c>
       <c r="U101" s="3">
-        <v>1.7649999999999999</v>
+        <f>T101-S101</f>
+        <v>1.7650000000000027E-3</v>
       </c>
       <c r="V101" s="3" t="s">
         <v>128</v>
@@ -9297,13 +9298,14 @@
         <v>128</v>
       </c>
       <c r="S102" s="3">
-        <v>33.628</v>
+        <v>3.3627999999999998E-2</v>
       </c>
       <c r="T102" s="3">
-        <v>36.954000000000001</v>
+        <v>3.6954000000000001E-2</v>
       </c>
       <c r="U102" s="3">
-        <v>3.3260000000000001</v>
+        <f t="shared" ref="U102:U165" si="9">T102-S102</f>
+        <v>3.3260000000000026E-3</v>
       </c>
       <c r="V102" s="3" t="s">
         <v>128</v>
@@ -9375,13 +9377,14 @@
         <v>128</v>
       </c>
       <c r="S103" s="3">
-        <v>34.343000000000004</v>
+        <v>3.4343000000000005E-2</v>
       </c>
       <c r="T103" s="3">
-        <v>35.325000000000003</v>
+        <v>3.5325000000000002E-2</v>
       </c>
       <c r="U103" s="3">
-        <v>0.98199999999999998</v>
+        <f t="shared" si="9"/>
+        <v>9.8199999999999676E-4</v>
       </c>
       <c r="V103" s="3" t="s">
         <v>128</v>
@@ -9453,13 +9456,14 @@
         <v>128</v>
       </c>
       <c r="S104" s="3">
-        <v>34.371000000000002</v>
+        <v>3.4370999999999999E-2</v>
       </c>
       <c r="T104" s="3">
-        <v>34.927</v>
+        <v>3.4927E-2</v>
       </c>
       <c r="U104" s="3">
-        <v>0.55600000000000005</v>
+        <f t="shared" si="9"/>
+        <v>5.5600000000000094E-4</v>
       </c>
       <c r="V104" s="3" t="s">
         <v>128</v>
@@ -9531,13 +9535,14 @@
         <v>128</v>
       </c>
       <c r="S105" s="3">
-        <v>34.162999999999997</v>
+        <v>3.4162999999999999E-2</v>
       </c>
       <c r="T105" s="3">
-        <v>38.170999999999999</v>
+        <v>3.8170999999999997E-2</v>
       </c>
       <c r="U105" s="3">
-        <v>4.008</v>
+        <f t="shared" si="9"/>
+        <v>4.0079999999999977E-3</v>
       </c>
       <c r="V105" s="3" t="s">
         <v>128</v>
@@ -9609,13 +9614,14 @@
         <v>128</v>
       </c>
       <c r="S106" s="3">
-        <v>33.174999999999997</v>
+        <v>3.3174999999999996E-2</v>
       </c>
       <c r="T106" s="3">
-        <v>33.793999999999997</v>
+        <v>3.3793999999999998E-2</v>
       </c>
       <c r="U106" s="3">
-        <v>0.61899999999999999</v>
+        <f t="shared" si="9"/>
+        <v>6.1900000000000149E-4</v>
       </c>
       <c r="V106" s="3" t="s">
         <v>128</v>
@@ -9687,13 +9693,14 @@
         <v>128</v>
       </c>
       <c r="S107" s="3">
-        <v>33.646000000000001</v>
+        <v>3.3646000000000002E-2</v>
       </c>
       <c r="T107" s="3">
-        <v>34.363999999999997</v>
+        <v>3.4363999999999999E-2</v>
       </c>
       <c r="U107" s="3">
-        <v>0.71799999999999997</v>
+        <f t="shared" si="9"/>
+        <v>7.1799999999999642E-4</v>
       </c>
       <c r="V107" s="3" t="s">
         <v>128</v>
@@ -9765,13 +9772,14 @@
         <v>128</v>
       </c>
       <c r="S108" s="3">
-        <v>35.174999999999997</v>
+        <v>3.5174999999999998E-2</v>
       </c>
       <c r="T108" s="3">
-        <v>35.545000000000002</v>
+        <v>3.5545E-2</v>
       </c>
       <c r="U108" s="3">
-        <v>0.37</v>
+        <f t="shared" si="9"/>
+        <v>3.7000000000000227E-4</v>
       </c>
       <c r="V108" s="3" t="s">
         <v>128</v>
@@ -9843,13 +9851,14 @@
         <v>128</v>
       </c>
       <c r="S109" s="3">
-        <v>33.237000000000002</v>
+        <v>3.3237000000000003E-2</v>
       </c>
       <c r="T109" s="3">
-        <v>35.180999999999997</v>
+        <v>3.5180999999999997E-2</v>
       </c>
       <c r="U109" s="3">
-        <v>1.944</v>
+        <f t="shared" si="9"/>
+        <v>1.9439999999999943E-3</v>
       </c>
       <c r="V109" s="3" t="s">
         <v>128</v>
@@ -9921,13 +9930,14 @@
         <v>128</v>
       </c>
       <c r="S110" s="3">
-        <v>32.840000000000003</v>
+        <v>3.2840000000000001E-2</v>
       </c>
       <c r="T110" s="3">
-        <v>33.709000000000003</v>
+        <v>3.3709000000000003E-2</v>
       </c>
       <c r="U110" s="3">
-        <v>0.86899999999999999</v>
+        <f t="shared" si="9"/>
+        <v>8.6900000000000172E-4</v>
       </c>
       <c r="V110" s="3" t="s">
         <v>128</v>
@@ -9999,13 +10009,14 @@
         <v>128</v>
       </c>
       <c r="S111" s="3">
-        <v>33.564999999999998</v>
+        <v>3.3564999999999998E-2</v>
       </c>
       <c r="T111" s="3">
-        <v>34.982999999999997</v>
+        <v>3.4983E-2</v>
       </c>
       <c r="U111" s="3">
-        <v>1.4179999999999999</v>
+        <f t="shared" si="9"/>
+        <v>1.4180000000000026E-3</v>
       </c>
       <c r="V111" s="3" t="s">
         <v>128</v>
@@ -10077,13 +10088,14 @@
         <v>128</v>
       </c>
       <c r="S112" s="3">
-        <v>33.165999999999997</v>
+        <v>3.3165999999999994E-2</v>
       </c>
       <c r="T112" s="3">
-        <v>35.350999999999999</v>
+        <v>3.5351E-2</v>
       </c>
       <c r="U112" s="3">
-        <v>2.1850000000000001</v>
+        <f t="shared" si="9"/>
+        <v>2.1850000000000064E-3</v>
       </c>
       <c r="V112" s="3" t="s">
         <v>128</v>
@@ -10155,13 +10167,14 @@
         <v>128</v>
       </c>
       <c r="S113" s="3">
-        <v>33.883000000000003</v>
+        <v>3.3883000000000003E-2</v>
       </c>
       <c r="T113" s="3">
-        <v>35.695</v>
+        <v>3.5694999999999998E-2</v>
       </c>
       <c r="U113" s="3">
-        <v>1.8120000000000001</v>
+        <f t="shared" si="9"/>
+        <v>1.8119999999999942E-3</v>
       </c>
       <c r="V113" s="3" t="s">
         <v>128</v>
@@ -10233,13 +10246,14 @@
         <v>128</v>
       </c>
       <c r="S114" s="3">
-        <v>34.603000000000002</v>
+        <v>3.4603000000000002E-2</v>
       </c>
       <c r="T114" s="3">
-        <v>35.335999999999999</v>
+        <v>3.5335999999999999E-2</v>
       </c>
       <c r="U114" s="3">
-        <v>0.73299999999999998</v>
+        <f t="shared" si="9"/>
+        <v>7.3299999999999754E-4</v>
       </c>
       <c r="V114" s="3" t="s">
         <v>128</v>
@@ -10311,13 +10325,14 @@
         <v>128</v>
       </c>
       <c r="S115" s="3">
-        <v>33.921999999999997</v>
+        <v>3.3921999999999994E-2</v>
       </c>
       <c r="T115" s="3">
-        <v>35.880000000000003</v>
+        <v>3.5880000000000002E-2</v>
       </c>
       <c r="U115" s="3">
-        <v>1.958</v>
+        <f t="shared" si="9"/>
+        <v>1.9580000000000083E-3</v>
       </c>
       <c r="V115" s="3" t="s">
         <v>128</v>
@@ -10389,13 +10404,14 @@
         <v>128</v>
       </c>
       <c r="S116" s="3">
-        <v>33.668999999999997</v>
+        <v>3.3668999999999998E-2</v>
       </c>
       <c r="T116" s="3">
-        <v>36.307000000000002</v>
+        <v>3.6306999999999999E-2</v>
       </c>
       <c r="U116" s="3">
-        <v>2.6379999999999999</v>
+        <f t="shared" si="9"/>
+        <v>2.6380000000000015E-3</v>
       </c>
       <c r="V116" s="3" t="s">
         <v>128</v>
@@ -10467,13 +10483,14 @@
         <v>128</v>
       </c>
       <c r="S117" s="3">
-        <v>33.945</v>
+        <v>3.3945000000000003E-2</v>
       </c>
       <c r="T117" s="3">
-        <v>35.323999999999998</v>
+        <v>3.5324000000000001E-2</v>
       </c>
       <c r="U117" s="3">
-        <v>1.379</v>
+        <f t="shared" si="9"/>
+        <v>1.3789999999999983E-3</v>
       </c>
       <c r="V117" s="3" t="s">
         <v>128</v>
@@ -10545,13 +10562,14 @@
         <v>128</v>
       </c>
       <c r="S118" s="3">
-        <v>32.637</v>
+        <v>3.2636999999999999E-2</v>
       </c>
       <c r="T118" s="3">
-        <v>33.457999999999998</v>
+        <v>3.3458000000000002E-2</v>
       </c>
       <c r="U118" s="3">
-        <v>0.82099999999999995</v>
+        <f t="shared" si="9"/>
+        <v>8.2100000000000228E-4</v>
       </c>
       <c r="V118" s="3" t="s">
         <v>128</v>
@@ -10623,13 +10641,14 @@
         <v>128</v>
       </c>
       <c r="S119" s="3">
-        <v>33.765000000000001</v>
+        <v>3.3765000000000003E-2</v>
       </c>
       <c r="T119" s="3">
-        <v>35.792999999999999</v>
+        <v>3.5792999999999998E-2</v>
       </c>
       <c r="U119" s="3">
-        <v>2.028</v>
+        <f t="shared" si="9"/>
+        <v>2.0279999999999951E-3</v>
       </c>
       <c r="V119" s="3" t="s">
         <v>128</v>
@@ -10701,13 +10720,14 @@
         <v>128</v>
       </c>
       <c r="S120" s="3">
-        <v>33.997999999999998</v>
+        <v>3.3998E-2</v>
       </c>
       <c r="T120" s="3">
-        <v>34.643999999999998</v>
+        <v>3.4644000000000001E-2</v>
       </c>
       <c r="U120" s="3">
-        <v>0.64600000000000002</v>
+        <f t="shared" si="9"/>
+        <v>6.4600000000000074E-4</v>
       </c>
       <c r="V120" s="3" t="s">
         <v>128</v>
@@ -10779,13 +10799,14 @@
         <v>128</v>
       </c>
       <c r="S121" s="3">
-        <v>33.613999999999997</v>
+        <v>3.3613999999999998E-2</v>
       </c>
       <c r="T121" s="3">
-        <v>34.189</v>
+        <v>3.4188999999999997E-2</v>
       </c>
       <c r="U121" s="3">
-        <v>0.57499999999999996</v>
+        <f t="shared" si="9"/>
+        <v>5.7499999999999912E-4</v>
       </c>
       <c r="V121" s="3" t="s">
         <v>128</v>
@@ -10857,7 +10878,7 @@
         <v>128</v>
       </c>
       <c r="S122" s="3">
-        <v>33.405999999999999</v>
+        <v>3.3405999999999998E-2</v>
       </c>
       <c r="T122" s="3" t="s">
         <v>128</v>
@@ -10935,13 +10956,14 @@
         <v>128</v>
       </c>
       <c r="S123" s="3">
-        <v>34.831000000000003</v>
+        <v>3.4831000000000001E-2</v>
       </c>
       <c r="T123" s="3">
-        <v>36.179000000000002</v>
+        <v>3.6179000000000003E-2</v>
       </c>
       <c r="U123" s="3">
-        <v>1.3480000000000001</v>
+        <f t="shared" si="9"/>
+        <v>1.348000000000002E-3</v>
       </c>
       <c r="V123" s="3" t="s">
         <v>128</v>
@@ -11013,13 +11035,14 @@
         <v>128</v>
       </c>
       <c r="S124" s="3">
-        <v>33.61</v>
+        <v>3.3610000000000001E-2</v>
       </c>
       <c r="T124" s="3">
-        <v>34.5</v>
+        <v>3.4500000000000003E-2</v>
       </c>
       <c r="U124" s="3">
-        <v>0.89</v>
+        <f t="shared" si="9"/>
+        <v>8.900000000000019E-4</v>
       </c>
       <c r="V124" s="3" t="s">
         <v>128</v>
@@ -11091,13 +11114,14 @@
         <v>128</v>
       </c>
       <c r="S125" s="3">
-        <v>34.146000000000001</v>
+        <v>3.4146000000000003E-2</v>
       </c>
       <c r="T125" s="3">
-        <v>34.545000000000002</v>
+        <v>3.4544999999999999E-2</v>
       </c>
       <c r="U125" s="3">
-        <v>0.39900000000000002</v>
+        <f t="shared" si="9"/>
+        <v>3.9899999999999658E-4</v>
       </c>
       <c r="V125" s="3" t="s">
         <v>128</v>
@@ -11169,13 +11193,14 @@
         <v>128</v>
       </c>
       <c r="S126" s="3">
-        <v>32.716000000000001</v>
+        <v>3.2716000000000002E-2</v>
       </c>
       <c r="T126" s="3">
-        <v>33.44</v>
+        <v>3.3439999999999998E-2</v>
       </c>
       <c r="U126" s="3">
-        <v>0.72399999999999998</v>
+        <f t="shared" si="9"/>
+        <v>7.2399999999999548E-4</v>
       </c>
       <c r="V126" s="3" t="s">
         <v>128</v>
@@ -11247,13 +11272,14 @@
         <v>128</v>
       </c>
       <c r="S127" s="3">
-        <v>34.728000000000002</v>
+        <v>3.4728000000000002E-2</v>
       </c>
       <c r="T127" s="3">
-        <v>36.435000000000002</v>
+        <v>3.6435000000000002E-2</v>
       </c>
       <c r="U127" s="3">
-        <v>1.7070000000000001</v>
+        <f t="shared" si="9"/>
+        <v>1.7070000000000002E-3</v>
       </c>
       <c r="V127" s="3" t="s">
         <v>128</v>
@@ -11325,13 +11351,14 @@
         <v>128</v>
       </c>
       <c r="S128" s="3">
-        <v>33.128</v>
+        <v>3.3127999999999998E-2</v>
       </c>
       <c r="T128" s="3">
-        <v>34.438000000000002</v>
+        <v>3.4438000000000003E-2</v>
       </c>
       <c r="U128" s="3">
-        <v>1.31</v>
+        <f t="shared" si="9"/>
+        <v>1.3100000000000056E-3</v>
       </c>
       <c r="V128" s="3" t="s">
         <v>128</v>
@@ -11403,13 +11430,14 @@
         <v>128</v>
       </c>
       <c r="S129" s="3">
-        <v>34.649000000000001</v>
+        <v>3.4648999999999999E-2</v>
       </c>
       <c r="T129" s="3">
-        <v>36.58</v>
+        <v>3.6580000000000001E-2</v>
       </c>
       <c r="U129" s="3">
-        <v>1.931</v>
+        <f t="shared" si="9"/>
+        <v>1.9310000000000022E-3</v>
       </c>
       <c r="V129" s="3" t="s">
         <v>128</v>
@@ -11481,13 +11509,14 @@
         <v>128</v>
       </c>
       <c r="S130" s="3">
-        <v>34.384999999999998</v>
+        <v>3.4384999999999999E-2</v>
       </c>
       <c r="T130" s="3">
-        <v>35.671999999999997</v>
+        <v>3.5671999999999995E-2</v>
       </c>
       <c r="U130" s="3">
-        <v>1.2869999999999999</v>
+        <f t="shared" si="9"/>
+        <v>1.2869999999999965E-3</v>
       </c>
       <c r="V130" s="3" t="s">
         <v>128</v>
@@ -11559,13 +11588,14 @@
         <v>128</v>
       </c>
       <c r="S131" s="3">
-        <v>32.933999999999997</v>
+        <v>3.2933999999999998E-2</v>
       </c>
       <c r="T131" s="3">
-        <v>34.756</v>
+        <v>3.4756000000000002E-2</v>
       </c>
       <c r="U131" s="3">
-        <v>1.8220000000000001</v>
+        <f t="shared" si="9"/>
+        <v>1.8220000000000042E-3</v>
       </c>
       <c r="V131" s="3" t="s">
         <v>128</v>
@@ -11637,13 +11667,14 @@
         <v>128</v>
       </c>
       <c r="S132" s="3">
-        <v>33.643999999999998</v>
+        <v>3.3644E-2</v>
       </c>
       <c r="T132" s="3">
-        <v>34.770000000000003</v>
+        <v>3.4770000000000002E-2</v>
       </c>
       <c r="U132" s="3">
-        <v>1.1259999999999999</v>
+        <f t="shared" si="9"/>
+        <v>1.126000000000002E-3</v>
       </c>
       <c r="V132" s="3" t="s">
         <v>128</v>
@@ -11715,13 +11746,14 @@
         <v>128</v>
       </c>
       <c r="S133" s="3">
-        <v>33.68</v>
+        <v>3.3680000000000002E-2</v>
       </c>
       <c r="T133" s="3">
-        <v>34.686999999999998</v>
+        <v>3.4686999999999996E-2</v>
       </c>
       <c r="U133" s="3">
-        <v>1.0069999999999999</v>
+        <f t="shared" si="9"/>
+        <v>1.006999999999994E-3</v>
       </c>
       <c r="V133" s="3" t="s">
         <v>128</v>
@@ -11793,13 +11825,14 @@
         <v>128</v>
       </c>
       <c r="S134" s="3">
-        <v>33.161999999999999</v>
+        <v>3.3161999999999997E-2</v>
       </c>
       <c r="T134" s="3">
-        <v>33.594999999999999</v>
+        <v>3.3595E-2</v>
       </c>
       <c r="U134" s="3">
-        <v>0.433</v>
+        <f t="shared" si="9"/>
+        <v>4.3300000000000283E-4</v>
       </c>
       <c r="V134" s="3" t="s">
         <v>128</v>
@@ -11871,13 +11904,14 @@
         <v>128</v>
       </c>
       <c r="S135" s="3">
-        <v>33.311</v>
+        <v>3.3311E-2</v>
       </c>
       <c r="T135" s="3">
-        <v>34.853000000000002</v>
+        <v>3.4853000000000002E-2</v>
       </c>
       <c r="U135" s="3">
-        <v>1.542</v>
+        <f t="shared" si="9"/>
+        <v>1.5420000000000017E-3</v>
       </c>
       <c r="V135" s="3" t="s">
         <v>128</v>
@@ -11949,13 +11983,14 @@
         <v>128</v>
       </c>
       <c r="S136" s="3">
-        <v>33.698999999999998</v>
+        <v>3.3699E-2</v>
       </c>
       <c r="T136" s="3">
-        <v>35.042000000000002</v>
+        <v>3.5042000000000004E-2</v>
       </c>
       <c r="U136" s="3">
-        <v>1.343</v>
+        <f t="shared" si="9"/>
+        <v>1.3430000000000039E-3</v>
       </c>
       <c r="V136" s="3" t="s">
         <v>128</v>
@@ -12027,13 +12062,14 @@
         <v>128</v>
       </c>
       <c r="S137" s="3">
-        <v>33.747</v>
+        <v>3.3746999999999999E-2</v>
       </c>
       <c r="T137" s="3">
-        <v>34.600999999999999</v>
+        <v>3.4601E-2</v>
       </c>
       <c r="U137" s="3">
-        <v>0.85399999999999998</v>
+        <f t="shared" si="9"/>
+        <v>8.5400000000000059E-4</v>
       </c>
       <c r="V137" s="3" t="s">
         <v>128</v>
@@ -12105,13 +12141,14 @@
         <v>128</v>
       </c>
       <c r="S138" s="3">
-        <v>33.137</v>
+        <v>3.3137E-2</v>
       </c>
       <c r="T138" s="3">
-        <v>34.008000000000003</v>
+        <v>3.4008000000000004E-2</v>
       </c>
       <c r="U138" s="3">
-        <v>0.871</v>
+        <f t="shared" si="9"/>
+        <v>8.7100000000000372E-4</v>
       </c>
       <c r="V138" s="3" t="s">
         <v>128</v>
@@ -12183,13 +12220,14 @@
         <v>128</v>
       </c>
       <c r="S139" s="3">
-        <v>33.387</v>
+        <v>3.3387E-2</v>
       </c>
       <c r="T139" s="3">
-        <v>34.731999999999999</v>
+        <v>3.4731999999999999E-2</v>
       </c>
       <c r="U139" s="3">
-        <v>1.345</v>
+        <f t="shared" si="9"/>
+        <v>1.344999999999999E-3</v>
       </c>
       <c r="V139" s="3" t="s">
         <v>128</v>
@@ -12261,13 +12299,14 @@
         <v>128</v>
       </c>
       <c r="S140" s="3">
-        <v>33.783999999999999</v>
+        <v>3.3784000000000002E-2</v>
       </c>
       <c r="T140" s="3">
-        <v>34.774999999999999</v>
+        <v>3.4775E-2</v>
       </c>
       <c r="U140" s="3">
-        <v>0.99099999999999999</v>
+        <f t="shared" si="9"/>
+        <v>9.9099999999999883E-4</v>
       </c>
       <c r="V140" s="3" t="s">
         <v>128</v>
@@ -12339,13 +12378,14 @@
         <v>128</v>
       </c>
       <c r="S141" s="3">
-        <v>33.942999999999998</v>
+        <v>3.3943000000000001E-2</v>
       </c>
       <c r="T141" s="3">
-        <v>35.081000000000003</v>
+        <v>3.5081000000000001E-2</v>
       </c>
       <c r="U141" s="3">
-        <v>1.1379999999999999</v>
+        <f t="shared" si="9"/>
+        <v>1.1380000000000001E-3</v>
       </c>
       <c r="V141" s="3" t="s">
         <v>128</v>
@@ -12417,13 +12457,14 @@
         <v>128</v>
       </c>
       <c r="S142" s="3">
-        <v>33.707000000000001</v>
+        <v>3.3707000000000001E-2</v>
       </c>
       <c r="T142" s="3">
-        <v>34.801000000000002</v>
+        <v>3.4800999999999999E-2</v>
       </c>
       <c r="U142" s="3">
-        <v>1.0940000000000001</v>
+        <f t="shared" si="9"/>
+        <v>1.0939999999999978E-3</v>
       </c>
       <c r="V142" s="3" t="s">
         <v>128</v>
@@ -12495,13 +12536,14 @@
         <v>128</v>
       </c>
       <c r="S143" s="3">
-        <v>33.536999999999999</v>
+        <v>3.3536999999999997E-2</v>
       </c>
       <c r="T143" s="3">
-        <v>33.865000000000002</v>
+        <v>3.3864999999999999E-2</v>
       </c>
       <c r="U143" s="3">
-        <v>0.32800000000000001</v>
+        <f t="shared" si="9"/>
+        <v>3.280000000000019E-4</v>
       </c>
       <c r="V143" s="3" t="s">
         <v>128</v>
@@ -12573,13 +12615,14 @@
         <v>128</v>
       </c>
       <c r="S144" s="3">
-        <v>33.786999999999999</v>
+        <v>3.3786999999999998E-2</v>
       </c>
       <c r="T144" s="3">
-        <v>37.774000000000001</v>
+        <v>3.7774000000000002E-2</v>
       </c>
       <c r="U144" s="3">
-        <v>3.9870000000000001</v>
+        <f t="shared" si="9"/>
+        <v>3.9870000000000044E-3</v>
       </c>
       <c r="V144" s="3" t="s">
         <v>128</v>
@@ -12651,13 +12694,14 @@
         <v>128</v>
       </c>
       <c r="S145" s="3">
-        <v>33.523000000000003</v>
+        <v>3.3523000000000004E-2</v>
       </c>
       <c r="T145" s="3">
-        <v>34.820999999999998</v>
+        <v>3.4820999999999998E-2</v>
       </c>
       <c r="U145" s="3">
-        <v>1.298</v>
+        <f t="shared" si="9"/>
+        <v>1.2979999999999936E-3</v>
       </c>
       <c r="V145" s="3" t="s">
         <v>128</v>
@@ -12729,13 +12773,14 @@
         <v>128</v>
       </c>
       <c r="S146" s="3">
-        <v>33.075000000000003</v>
+        <v>3.3075E-2</v>
       </c>
       <c r="T146" s="3">
-        <v>33.963000000000001</v>
+        <v>3.3963E-2</v>
       </c>
       <c r="U146" s="3">
-        <v>0.88800000000000001</v>
+        <f t="shared" si="9"/>
+        <v>8.879999999999999E-4</v>
       </c>
       <c r="V146" s="3" t="s">
         <v>128</v>
@@ -12807,13 +12852,14 @@
         <v>128</v>
       </c>
       <c r="S147" s="3">
-        <v>33.567</v>
+        <v>3.3567E-2</v>
       </c>
       <c r="T147" s="3">
-        <v>33.972999999999999</v>
+        <v>3.3972999999999996E-2</v>
       </c>
       <c r="U147" s="3">
-        <v>0.40600000000000003</v>
+        <f t="shared" si="9"/>
+        <v>4.0599999999999664E-4</v>
       </c>
       <c r="V147" s="3" t="s">
         <v>128</v>
@@ -12885,13 +12931,14 @@
         <v>128</v>
       </c>
       <c r="S148" s="3">
-        <v>33.476999999999997</v>
+        <v>3.3477E-2</v>
       </c>
       <c r="T148" s="3">
-        <v>33.851999999999997</v>
+        <v>3.3852E-2</v>
       </c>
       <c r="U148" s="3">
-        <v>0.375</v>
+        <f t="shared" si="9"/>
+        <v>3.7500000000000033E-4</v>
       </c>
       <c r="V148" s="3" t="s">
         <v>128</v>
@@ -12963,13 +13010,14 @@
         <v>128</v>
       </c>
       <c r="S149" s="3">
-        <v>33.81</v>
+        <v>3.381E-2</v>
       </c>
       <c r="T149" s="3">
-        <v>34.405999999999999</v>
+        <v>3.4405999999999999E-2</v>
       </c>
       <c r="U149" s="3">
-        <v>0.59599999999999997</v>
+        <f t="shared" si="9"/>
+        <v>5.9599999999999931E-4</v>
       </c>
       <c r="V149" s="3" t="s">
         <v>128</v>
@@ -13041,13 +13089,14 @@
         <v>128</v>
       </c>
       <c r="S150" s="3">
-        <v>33.976999999999997</v>
+        <v>3.3976999999999993E-2</v>
       </c>
       <c r="T150" s="3">
-        <v>34.750999999999998</v>
+        <v>3.4750999999999997E-2</v>
       </c>
       <c r="U150" s="3">
-        <v>0.77400000000000002</v>
+        <f t="shared" si="9"/>
+        <v>7.7400000000000385E-4</v>
       </c>
       <c r="V150" s="3" t="s">
         <v>128</v>
@@ -13119,13 +13168,14 @@
         <v>128</v>
       </c>
       <c r="S151" s="3">
-        <v>33.450000000000003</v>
+        <v>3.3450000000000001E-2</v>
       </c>
       <c r="T151" s="3">
-        <v>33.676000000000002</v>
+        <v>3.3676000000000005E-2</v>
       </c>
       <c r="U151" s="3">
-        <v>0.22600000000000001</v>
+        <f t="shared" si="9"/>
+        <v>2.2600000000000398E-4</v>
       </c>
       <c r="V151" s="3" t="s">
         <v>128</v>
@@ -13197,13 +13247,14 @@
         <v>128</v>
       </c>
       <c r="S152" s="3">
-        <v>33.421999999999997</v>
+        <v>3.3422E-2</v>
       </c>
       <c r="T152" s="3">
-        <v>34.51</v>
+        <v>3.4509999999999999E-2</v>
       </c>
       <c r="U152" s="3">
-        <v>1.0880000000000001</v>
+        <f t="shared" si="9"/>
+        <v>1.0879999999999987E-3</v>
       </c>
       <c r="V152" s="3" t="s">
         <v>128</v>
@@ -13275,13 +13326,14 @@
         <v>128</v>
       </c>
       <c r="S153" s="3">
-        <v>33.704000000000001</v>
+        <v>3.3703999999999998E-2</v>
       </c>
       <c r="T153" s="3">
-        <v>34.253999999999998</v>
+        <v>3.4254E-2</v>
       </c>
       <c r="U153" s="3">
-        <v>0.55000000000000004</v>
+        <f t="shared" si="9"/>
+        <v>5.5000000000000188E-4</v>
       </c>
       <c r="V153" s="3" t="s">
         <v>128</v>
@@ -13353,13 +13405,14 @@
         <v>128</v>
       </c>
       <c r="S154" s="3">
-        <v>33.524999999999999</v>
+        <v>3.3524999999999999E-2</v>
       </c>
       <c r="T154" s="3">
-        <v>33.798999999999999</v>
+        <v>3.3799000000000003E-2</v>
       </c>
       <c r="U154" s="3">
-        <v>0.27400000000000002</v>
+        <f t="shared" si="9"/>
+        <v>2.7400000000000341E-4</v>
       </c>
       <c r="V154" s="3" t="s">
         <v>128</v>
@@ -13431,13 +13484,14 @@
         <v>128</v>
       </c>
       <c r="S155" s="3">
-        <v>33.726999999999997</v>
+        <v>3.3727E-2</v>
       </c>
       <c r="T155" s="3">
-        <v>34.491999999999997</v>
+        <v>3.4491999999999995E-2</v>
       </c>
       <c r="U155" s="3">
-        <v>0.76500000000000001</v>
+        <f t="shared" si="9"/>
+        <v>7.6499999999999485E-4</v>
       </c>
       <c r="V155" s="3" t="s">
         <v>128</v>
@@ -13509,13 +13563,14 @@
         <v>128</v>
       </c>
       <c r="S156" s="3">
-        <v>33.664000000000001</v>
+        <v>3.3663999999999999E-2</v>
       </c>
       <c r="T156" s="3">
-        <v>34.268999999999998</v>
+        <v>3.4269000000000001E-2</v>
       </c>
       <c r="U156" s="3">
-        <v>0.60499999999999998</v>
+        <f t="shared" si="9"/>
+        <v>6.0500000000000137E-4</v>
       </c>
       <c r="V156" s="3" t="s">
         <v>128</v>
@@ -13587,13 +13642,14 @@
         <v>128</v>
       </c>
       <c r="S157" s="3">
-        <v>33.295000000000002</v>
+        <v>3.3295000000000005E-2</v>
       </c>
       <c r="T157" s="3">
-        <v>34.134999999999998</v>
+        <v>3.4134999999999999E-2</v>
       </c>
       <c r="U157" s="3">
-        <v>0.84</v>
+        <f t="shared" si="9"/>
+        <v>8.3999999999999353E-4</v>
       </c>
       <c r="V157" s="3" t="s">
         <v>128</v>
@@ -13665,13 +13721,14 @@
         <v>128</v>
       </c>
       <c r="S158" s="3">
-        <v>33.896999999999998</v>
+        <v>3.3896999999999997E-2</v>
       </c>
       <c r="T158" s="3">
-        <v>34.935000000000002</v>
+        <v>3.4935000000000001E-2</v>
       </c>
       <c r="U158" s="3">
-        <v>1.038</v>
+        <f t="shared" si="9"/>
+        <v>1.0380000000000042E-3</v>
       </c>
       <c r="V158" s="3" t="s">
         <v>128</v>
@@ -13743,13 +13800,14 @@
         <v>128</v>
       </c>
       <c r="S159" s="3">
-        <v>33.302</v>
+        <v>3.3301999999999998E-2</v>
       </c>
       <c r="T159" s="3">
-        <v>33.947000000000003</v>
+        <v>3.3947000000000005E-2</v>
       </c>
       <c r="U159" s="3">
-        <v>0.64500000000000002</v>
+        <f t="shared" si="9"/>
+        <v>6.4500000000000668E-4</v>
       </c>
       <c r="V159" s="3" t="s">
         <v>128</v>
@@ -13821,13 +13879,14 @@
         <v>128</v>
       </c>
       <c r="S160" s="3">
-        <v>34.106999999999999</v>
+        <v>3.4106999999999998E-2</v>
       </c>
       <c r="T160" s="3">
-        <v>34.738</v>
+        <v>3.4737999999999998E-2</v>
       </c>
       <c r="U160" s="3">
-        <v>0.63100000000000001</v>
+        <f t="shared" si="9"/>
+        <v>6.3099999999999962E-4</v>
       </c>
       <c r="V160" s="3" t="s">
         <v>128</v>
@@ -13899,13 +13958,14 @@
         <v>128</v>
       </c>
       <c r="S161" s="3">
-        <v>34.686999999999998</v>
+        <v>3.4686999999999996E-2</v>
       </c>
       <c r="T161" s="3">
-        <v>37.468000000000004</v>
+        <v>3.7468000000000001E-2</v>
       </c>
       <c r="U161" s="3">
-        <v>2.7810000000000001</v>
+        <f t="shared" si="9"/>
+        <v>2.7810000000000057E-3</v>
       </c>
       <c r="V161" s="3" t="s">
         <v>128</v>
@@ -13977,13 +14037,14 @@
         <v>128</v>
       </c>
       <c r="S162" s="3">
-        <v>33.893999999999998</v>
+        <v>3.3894000000000001E-2</v>
       </c>
       <c r="T162" s="3">
-        <v>34.963000000000001</v>
+        <v>3.4963000000000001E-2</v>
       </c>
       <c r="U162" s="3">
-        <v>1.069</v>
+        <f t="shared" si="9"/>
+        <v>1.0690000000000005E-3</v>
       </c>
       <c r="V162" s="3" t="s">
         <v>128</v>
@@ -14055,13 +14116,14 @@
         <v>128</v>
       </c>
       <c r="S163" s="3">
-        <v>32.734000000000002</v>
+        <v>3.2733999999999999E-2</v>
       </c>
       <c r="T163" s="3">
-        <v>33.58</v>
+        <v>3.3579999999999999E-2</v>
       </c>
       <c r="U163" s="3">
-        <v>0.84599999999999997</v>
+        <f t="shared" si="9"/>
+        <v>8.4599999999999953E-4</v>
       </c>
       <c r="V163" s="3" t="s">
         <v>128</v>
@@ -14133,13 +14195,14 @@
         <v>128</v>
       </c>
       <c r="S164" s="3">
-        <v>34.286000000000001</v>
+        <v>3.4286000000000004E-2</v>
       </c>
       <c r="T164" s="3">
-        <v>35.704000000000001</v>
+        <v>3.5704E-2</v>
       </c>
       <c r="U164" s="3">
-        <v>1.4179999999999999</v>
+        <f t="shared" si="9"/>
+        <v>1.4179999999999957E-3</v>
       </c>
       <c r="V164" s="3" t="s">
         <v>128</v>
@@ -14211,13 +14274,14 @@
         <v>128</v>
       </c>
       <c r="S165" s="3">
-        <v>32.954000000000001</v>
+        <v>3.2953999999999997E-2</v>
       </c>
       <c r="T165" s="3">
-        <v>33.359000000000002</v>
+        <v>3.3359E-2</v>
       </c>
       <c r="U165" s="3">
-        <v>0.40500000000000003</v>
+        <f t="shared" si="9"/>
+        <v>4.0500000000000258E-4</v>
       </c>
       <c r="V165" s="3" t="s">
         <v>128</v>
@@ -14289,13 +14353,14 @@
         <v>128</v>
       </c>
       <c r="S166" s="3">
-        <v>32.99</v>
+        <v>3.2990000000000005E-2</v>
       </c>
       <c r="T166" s="3">
-        <v>34.037999999999997</v>
+        <v>3.4037999999999999E-2</v>
       </c>
       <c r="U166" s="3">
-        <v>1.048</v>
+        <f t="shared" ref="U166:U229" si="10">T166-S166</f>
+        <v>1.0479999999999934E-3</v>
       </c>
       <c r="V166" s="3" t="s">
         <v>128</v>
@@ -14367,13 +14432,14 @@
         <v>128</v>
       </c>
       <c r="S167" s="3">
-        <v>34.043999999999997</v>
+        <v>3.4043999999999998E-2</v>
       </c>
       <c r="T167" s="3">
-        <v>36.460999999999999</v>
+        <v>3.6461E-2</v>
       </c>
       <c r="U167" s="3">
-        <v>2.4169999999999998</v>
+        <f t="shared" si="10"/>
+        <v>2.4170000000000025E-3</v>
       </c>
       <c r="V167" s="3" t="s">
         <v>128</v>
@@ -14445,13 +14511,14 @@
         <v>128</v>
       </c>
       <c r="S168" s="3">
-        <v>34.219000000000001</v>
+        <v>3.4218999999999999E-2</v>
       </c>
       <c r="T168" s="3">
-        <v>34.365000000000002</v>
+        <v>3.4365E-2</v>
       </c>
       <c r="U168" s="3">
-        <v>0.14599999999999999</v>
+        <f t="shared" si="10"/>
+        <v>1.460000000000003E-4</v>
       </c>
       <c r="V168" s="3" t="s">
         <v>128</v>
@@ -14523,13 +14590,14 @@
         <v>128</v>
       </c>
       <c r="S169" s="3">
-        <v>32.945</v>
+        <v>3.2945000000000002E-2</v>
       </c>
       <c r="T169" s="3">
-        <v>35.273000000000003</v>
+        <v>3.5273000000000006E-2</v>
       </c>
       <c r="U169" s="3">
-        <v>2.3279999999999998</v>
+        <f t="shared" si="10"/>
+        <v>2.3280000000000037E-3</v>
       </c>
       <c r="V169" s="3" t="s">
         <v>128</v>
@@ -14601,13 +14669,14 @@
         <v>128</v>
       </c>
       <c r="S170" s="3">
-        <v>33.777000000000001</v>
+        <v>3.3777000000000001E-2</v>
       </c>
       <c r="T170" s="3">
-        <v>34.395000000000003</v>
+        <v>3.4395000000000002E-2</v>
       </c>
       <c r="U170" s="3">
-        <v>0.61799999999999999</v>
+        <f t="shared" si="10"/>
+        <v>6.1800000000000049E-4</v>
       </c>
       <c r="V170" s="3" t="s">
         <v>128</v>
@@ -14679,13 +14748,14 @@
         <v>128</v>
       </c>
       <c r="S171" s="3">
-        <v>34.142000000000003</v>
+        <v>3.4142000000000006E-2</v>
       </c>
       <c r="T171" s="3">
-        <v>38.290999999999997</v>
+        <v>3.8290999999999999E-2</v>
       </c>
       <c r="U171" s="3">
-        <v>4.149</v>
+        <f t="shared" si="10"/>
+        <v>4.148999999999993E-3</v>
       </c>
       <c r="V171" s="3" t="s">
         <v>128</v>
@@ -14756,13 +14826,14 @@
         <v>128</v>
       </c>
       <c r="S172" s="3">
-        <v>34.118000000000002</v>
+        <v>3.4118000000000002E-2</v>
       </c>
       <c r="T172" s="3">
-        <v>38.981000000000002</v>
+        <v>3.8981000000000002E-2</v>
       </c>
       <c r="U172" s="3">
-        <v>4.8630000000000004</v>
+        <f t="shared" si="10"/>
+        <v>4.8629999999999993E-3</v>
       </c>
       <c r="V172" s="3" t="s">
         <v>128</v>
@@ -14833,13 +14904,14 @@
         <v>128</v>
       </c>
       <c r="S173" s="3">
-        <v>34.625</v>
+        <v>3.4625000000000003E-2</v>
       </c>
       <c r="T173" s="3">
-        <v>36.933</v>
+        <v>3.6933000000000001E-2</v>
       </c>
       <c r="U173" s="3">
-        <v>2.3079999999999998</v>
+        <f t="shared" si="10"/>
+        <v>2.3079999999999976E-3</v>
       </c>
       <c r="V173" s="3" t="s">
         <v>128</v>
@@ -14910,13 +14982,14 @@
         <v>128</v>
       </c>
       <c r="S174" s="3">
-        <v>33.472000000000001</v>
+        <v>3.3472000000000002E-2</v>
       </c>
       <c r="T174" s="3">
-        <v>45.091000000000001</v>
+        <v>4.5090999999999999E-2</v>
       </c>
       <c r="U174" s="3">
-        <v>11.619</v>
+        <f t="shared" si="10"/>
+        <v>1.1618999999999997E-2</v>
       </c>
       <c r="V174" s="3" t="s">
         <v>128</v>
@@ -14987,13 +15060,14 @@
         <v>128</v>
       </c>
       <c r="S175" s="3">
-        <v>34.414999999999999</v>
+        <v>3.4415000000000001E-2</v>
       </c>
       <c r="T175" s="3">
-        <v>37.725000000000001</v>
+        <v>3.7725000000000002E-2</v>
       </c>
       <c r="U175" s="3">
-        <v>3.31</v>
+        <f t="shared" si="10"/>
+        <v>3.3100000000000004E-3</v>
       </c>
       <c r="V175" s="3" t="s">
         <v>128</v>
@@ -15064,13 +15138,14 @@
         <v>128</v>
       </c>
       <c r="S176" s="3">
-        <v>33.33</v>
+        <v>3.3329999999999999E-2</v>
       </c>
       <c r="T176" s="3">
-        <v>47.064</v>
+        <v>4.7064000000000002E-2</v>
       </c>
       <c r="U176" s="3">
-        <v>13.734</v>
+        <f t="shared" si="10"/>
+        <v>1.3734000000000003E-2</v>
       </c>
       <c r="V176" s="3" t="s">
         <v>128</v>
@@ -15141,13 +15216,14 @@
         <v>128</v>
       </c>
       <c r="S177" s="3">
-        <v>33.911000000000001</v>
+        <v>3.3911000000000004E-2</v>
       </c>
       <c r="T177" s="3">
-        <v>35.122</v>
+        <v>3.5122E-2</v>
       </c>
       <c r="U177" s="3">
-        <v>1.2110000000000001</v>
+        <f t="shared" si="10"/>
+        <v>1.2109999999999968E-3</v>
       </c>
       <c r="V177" s="3" t="s">
         <v>128</v>
@@ -15218,13 +15294,14 @@
         <v>128</v>
       </c>
       <c r="S178" s="3">
-        <v>32.734999999999999</v>
+        <v>3.2735E-2</v>
       </c>
       <c r="T178" s="3">
-        <v>37.933</v>
+        <v>3.7933000000000001E-2</v>
       </c>
       <c r="U178" s="3">
-        <v>5.1980000000000004</v>
+        <f t="shared" si="10"/>
+        <v>5.1980000000000012E-3</v>
       </c>
       <c r="V178" s="3" t="s">
         <v>128</v>
@@ -15295,13 +15372,14 @@
         <v>128</v>
       </c>
       <c r="S179" s="3">
-        <v>34.548999999999999</v>
+        <v>3.4548999999999996E-2</v>
       </c>
       <c r="T179" s="3">
-        <v>35.587000000000003</v>
+        <v>3.5587000000000001E-2</v>
       </c>
       <c r="U179" s="3">
-        <v>1.038</v>
+        <f t="shared" si="10"/>
+        <v>1.0380000000000042E-3</v>
       </c>
       <c r="V179" s="3" t="s">
         <v>128</v>
@@ -15372,13 +15450,14 @@
         <v>128</v>
       </c>
       <c r="S180" s="3">
-        <v>33.32</v>
+        <v>3.3320000000000002E-2</v>
       </c>
       <c r="T180" s="3">
-        <v>34.701999999999998</v>
+        <v>3.4701999999999997E-2</v>
       </c>
       <c r="U180" s="3">
-        <v>1.3819999999999999</v>
+        <f t="shared" si="10"/>
+        <v>1.3819999999999943E-3</v>
       </c>
       <c r="V180" s="3" t="s">
         <v>128</v>
@@ -15449,13 +15528,14 @@
         <v>128</v>
       </c>
       <c r="S181" s="3">
-        <v>32.896000000000001</v>
+        <v>3.2896000000000002E-2</v>
       </c>
       <c r="T181" s="3">
-        <v>38.466999999999999</v>
+        <v>3.8467000000000001E-2</v>
       </c>
       <c r="U181" s="3">
-        <v>5.5709999999999997</v>
+        <f t="shared" si="10"/>
+        <v>5.5709999999999996E-3</v>
       </c>
       <c r="V181" s="3" t="s">
         <v>128</v>
@@ -15526,13 +15606,14 @@
         <v>128</v>
       </c>
       <c r="S182" s="3">
-        <v>33.54</v>
+        <v>3.354E-2</v>
       </c>
       <c r="T182" s="3">
-        <v>38.344999999999999</v>
+        <v>3.8344999999999997E-2</v>
       </c>
       <c r="U182" s="3">
-        <v>4.8049999999999997</v>
+        <f t="shared" si="10"/>
+        <v>4.8049999999999968E-3</v>
       </c>
       <c r="V182" s="3" t="s">
         <v>128</v>
@@ -15603,13 +15684,14 @@
         <v>128</v>
       </c>
       <c r="S183" s="3">
-        <v>33.366</v>
+        <v>3.3366E-2</v>
       </c>
       <c r="T183" s="3">
-        <v>36.393000000000001</v>
+        <v>3.6393000000000002E-2</v>
       </c>
       <c r="U183" s="3">
-        <v>3.0270000000000001</v>
+        <f t="shared" si="10"/>
+        <v>3.0270000000000019E-3</v>
       </c>
       <c r="V183" s="3" t="s">
         <v>128</v>
@@ -15680,13 +15762,14 @@
         <v>128</v>
       </c>
       <c r="S184" s="3">
-        <v>34.301000000000002</v>
+        <v>3.4301000000000005E-2</v>
       </c>
       <c r="T184" s="3">
-        <v>38.668999999999997</v>
+        <v>3.8668999999999995E-2</v>
       </c>
       <c r="U184" s="3">
-        <v>4.3680000000000003</v>
+        <f t="shared" si="10"/>
+        <v>4.3679999999999899E-3</v>
       </c>
       <c r="V184" s="3" t="s">
         <v>128</v>
@@ -15757,13 +15840,14 @@
         <v>128</v>
       </c>
       <c r="S185" s="3">
-        <v>34.527000000000001</v>
+        <v>3.4527000000000002E-2</v>
       </c>
       <c r="T185" s="3">
-        <v>38.475000000000001</v>
+        <v>3.8475000000000002E-2</v>
       </c>
       <c r="U185" s="3">
-        <v>3.948</v>
+        <f t="shared" si="10"/>
+        <v>3.9480000000000001E-3</v>
       </c>
       <c r="V185" s="3" t="s">
         <v>128</v>
@@ -15834,13 +15918,14 @@
         <v>128</v>
       </c>
       <c r="S186" s="3">
-        <v>33.325000000000003</v>
+        <v>3.3325E-2</v>
       </c>
       <c r="T186" s="3">
-        <v>34.636000000000003</v>
+        <v>3.4636E-2</v>
       </c>
       <c r="U186" s="3">
-        <v>1.3109999999999999</v>
+        <f t="shared" si="10"/>
+        <v>1.3109999999999997E-3</v>
       </c>
       <c r="V186" s="3" t="s">
         <v>128</v>
@@ -15911,13 +15996,14 @@
         <v>128</v>
       </c>
       <c r="S187" s="3">
-        <v>32.405999999999999</v>
+        <v>3.2405999999999997E-2</v>
       </c>
       <c r="T187" s="3">
-        <v>34.44</v>
+        <v>3.4439999999999998E-2</v>
       </c>
       <c r="U187" s="3">
-        <v>2.0339999999999998</v>
+        <f t="shared" si="10"/>
+        <v>2.0340000000000011E-3</v>
       </c>
       <c r="V187" s="3" t="s">
         <v>128</v>
@@ -15988,13 +16074,14 @@
         <v>128</v>
       </c>
       <c r="S188" s="3">
-        <v>33.304000000000002</v>
+        <v>3.3304E-2</v>
       </c>
       <c r="T188" s="3">
-        <v>34.131999999999998</v>
+        <v>3.4131999999999996E-2</v>
       </c>
       <c r="U188" s="3">
-        <v>0.82799999999999996</v>
+        <f t="shared" si="10"/>
+        <v>8.2799999999999541E-4</v>
       </c>
       <c r="V188" s="3" t="s">
         <v>128</v>
@@ -16065,13 +16152,14 @@
         <v>128</v>
       </c>
       <c r="S189" s="3">
-        <v>31.879000000000001</v>
+        <v>3.1879000000000005E-2</v>
       </c>
       <c r="T189" s="3">
-        <v>35.695999999999998</v>
+        <v>3.5695999999999999E-2</v>
       </c>
       <c r="U189" s="3">
-        <v>3.8170000000000002</v>
+        <f t="shared" si="10"/>
+        <v>3.816999999999994E-3</v>
       </c>
       <c r="V189" s="3" t="s">
         <v>128</v>
@@ -16142,13 +16230,14 @@
         <v>128</v>
       </c>
       <c r="S190" s="3">
-        <v>34.636000000000003</v>
+        <v>3.4636E-2</v>
       </c>
       <c r="T190" s="3">
-        <v>36.540999999999997</v>
+        <v>3.6540999999999997E-2</v>
       </c>
       <c r="U190" s="3">
-        <v>1.905</v>
+        <f t="shared" si="10"/>
+        <v>1.904999999999997E-3</v>
       </c>
       <c r="V190" s="3" t="s">
         <v>128</v>
@@ -16219,13 +16308,14 @@
         <v>128</v>
       </c>
       <c r="S191" s="3">
-        <v>34.250999999999998</v>
+        <v>3.4250999999999997E-2</v>
       </c>
       <c r="T191" s="3">
-        <v>35.046999999999997</v>
+        <v>3.5046999999999995E-2</v>
       </c>
       <c r="U191" s="3">
-        <v>0.79600000000000004</v>
+        <f t="shared" si="10"/>
+        <v>7.959999999999981E-4</v>
       </c>
       <c r="V191" s="3" t="s">
         <v>128</v>
@@ -16296,13 +16386,14 @@
         <v>128</v>
       </c>
       <c r="S192" s="3">
-        <v>33.74</v>
+        <v>3.3739999999999999E-2</v>
       </c>
       <c r="T192" s="3">
-        <v>38.023000000000003</v>
+        <v>3.8023000000000001E-2</v>
       </c>
       <c r="U192" s="3">
-        <v>4.2830000000000004</v>
+        <f t="shared" si="10"/>
+        <v>4.2830000000000021E-3</v>
       </c>
       <c r="V192" s="3" t="s">
         <v>128</v>
@@ -16373,13 +16464,14 @@
         <v>128</v>
       </c>
       <c r="S193" s="3">
-        <v>33.167000000000002</v>
+        <v>3.3167000000000002E-2</v>
       </c>
       <c r="T193" s="3">
-        <v>33.768999999999998</v>
+        <v>3.3769E-2</v>
       </c>
       <c r="U193" s="3">
-        <v>0.60199999999999998</v>
+        <f t="shared" si="10"/>
+        <v>6.0199999999999837E-4</v>
       </c>
       <c r="V193" s="3" t="s">
         <v>128</v>
@@ -16450,13 +16542,14 @@
         <v>128</v>
       </c>
       <c r="S194" s="3">
-        <v>33.524999999999999</v>
+        <v>3.3524999999999999E-2</v>
       </c>
       <c r="T194" s="3">
-        <v>35.968000000000004</v>
+        <v>3.5968000000000007E-2</v>
       </c>
       <c r="U194" s="3">
-        <v>2.4430000000000001</v>
+        <f t="shared" si="10"/>
+        <v>2.4430000000000077E-3</v>
       </c>
       <c r="V194" s="3" t="s">
         <v>128</v>
@@ -16527,13 +16620,14 @@
         <v>128</v>
       </c>
       <c r="S195" s="3">
-        <v>33.040999999999997</v>
+        <v>3.3040999999999994E-2</v>
       </c>
       <c r="T195" s="3">
-        <v>34.502000000000002</v>
+        <v>3.4502000000000005E-2</v>
       </c>
       <c r="U195" s="3">
-        <v>1.4610000000000001</v>
+        <f t="shared" si="10"/>
+        <v>1.4610000000000109E-3</v>
       </c>
       <c r="V195" s="3" t="s">
         <v>128</v>
@@ -16604,13 +16698,14 @@
         <v>128</v>
       </c>
       <c r="S196" s="3">
-        <v>33.554000000000002</v>
+        <v>3.3554E-2</v>
       </c>
       <c r="T196" s="3">
-        <v>37.707000000000001</v>
+        <v>3.7706999999999997E-2</v>
       </c>
       <c r="U196" s="3">
-        <v>4.1529999999999996</v>
+        <f t="shared" si="10"/>
+        <v>4.152999999999997E-3</v>
       </c>
       <c r="V196" s="3" t="s">
         <v>128</v>
@@ -16681,13 +16776,14 @@
         <v>128</v>
       </c>
       <c r="S197" s="3">
-        <v>34.142000000000003</v>
+        <v>3.4142000000000006E-2</v>
       </c>
       <c r="T197" s="3">
-        <v>41.932000000000002</v>
+        <v>4.1932000000000004E-2</v>
       </c>
       <c r="U197" s="3">
-        <v>7.79</v>
+        <f t="shared" si="10"/>
+        <v>7.7899999999999983E-3</v>
       </c>
       <c r="V197" s="3" t="s">
         <v>128</v>
@@ -16758,13 +16854,14 @@
         <v>128</v>
       </c>
       <c r="S198" s="3">
-        <v>32.920999999999999</v>
+        <v>3.2920999999999999E-2</v>
       </c>
       <c r="T198" s="3">
-        <v>34.042999999999999</v>
+        <v>3.4042999999999997E-2</v>
       </c>
       <c r="U198" s="3">
-        <v>1.1220000000000001</v>
+        <f t="shared" si="10"/>
+        <v>1.121999999999998E-3</v>
       </c>
       <c r="V198" s="3" t="s">
         <v>128</v>
@@ -16835,13 +16932,14 @@
         <v>128</v>
       </c>
       <c r="S199" s="3">
-        <v>33.082000000000001</v>
+        <v>3.3082E-2</v>
       </c>
       <c r="T199" s="3">
-        <v>35.308999999999997</v>
+        <v>3.5309E-2</v>
       </c>
       <c r="U199" s="3">
-        <v>2.2269999999999999</v>
+        <f t="shared" si="10"/>
+        <v>2.2269999999999998E-3</v>
       </c>
       <c r="V199" s="3" t="s">
         <v>128</v>
@@ -16912,13 +17010,14 @@
         <v>128</v>
       </c>
       <c r="S200" s="3">
-        <v>34.643999999999998</v>
+        <v>3.4644000000000001E-2</v>
       </c>
       <c r="T200" s="3">
-        <v>36.011000000000003</v>
+        <v>3.6011000000000001E-2</v>
       </c>
       <c r="U200" s="3">
-        <v>1.367</v>
+        <f t="shared" si="10"/>
+        <v>1.3670000000000002E-3</v>
       </c>
       <c r="V200" s="3" t="s">
         <v>128</v>
@@ -16989,13 +17088,14 @@
         <v>128</v>
       </c>
       <c r="S201" s="3">
-        <v>34.503</v>
+        <v>3.4502999999999999E-2</v>
       </c>
       <c r="T201" s="3">
-        <v>36.155000000000001</v>
+        <v>3.6155E-2</v>
       </c>
       <c r="U201" s="3">
-        <v>1.6519999999999999</v>
+        <f t="shared" si="10"/>
+        <v>1.6520000000000007E-3</v>
       </c>
       <c r="V201" s="3" t="s">
         <v>128</v>
@@ -17066,13 +17166,14 @@
         <v>128</v>
       </c>
       <c r="S202" s="3">
-        <v>33.195999999999998</v>
+        <v>3.3195999999999996E-2</v>
       </c>
       <c r="T202" s="3">
-        <v>35.058</v>
+        <v>3.5057999999999999E-2</v>
       </c>
       <c r="U202" s="3">
-        <v>1.8620000000000001</v>
+        <f t="shared" si="10"/>
+        <v>1.8620000000000025E-3</v>
       </c>
       <c r="V202" s="3" t="s">
         <v>128</v>
@@ -17143,13 +17244,14 @@
         <v>128</v>
       </c>
       <c r="S203" s="3">
-        <v>34.692999999999998</v>
+        <v>3.4692999999999995E-2</v>
       </c>
       <c r="T203" s="3">
-        <v>39.686999999999998</v>
+        <v>3.9687E-2</v>
       </c>
       <c r="U203" s="3">
-        <v>4.9939999999999998</v>
+        <f t="shared" si="10"/>
+        <v>4.9940000000000054E-3</v>
       </c>
       <c r="V203" s="3" t="s">
         <v>128</v>
@@ -17220,13 +17322,14 @@
         <v>128</v>
       </c>
       <c r="S204" s="3">
-        <v>32.975000000000001</v>
+        <v>3.2975000000000004E-2</v>
       </c>
       <c r="T204" s="3">
-        <v>44.470999999999997</v>
+        <v>4.4470999999999997E-2</v>
       </c>
       <c r="U204" s="3">
-        <v>11.496</v>
+        <f t="shared" si="10"/>
+        <v>1.1495999999999992E-2</v>
       </c>
       <c r="V204" s="3" t="s">
         <v>128</v>
@@ -17297,13 +17400,14 @@
         <v>128</v>
       </c>
       <c r="S205" s="3">
-        <v>33.652999999999999</v>
+        <v>3.3652999999999995E-2</v>
       </c>
       <c r="T205" s="3">
-        <v>35.667000000000002</v>
+        <v>3.5667000000000004E-2</v>
       </c>
       <c r="U205" s="3">
-        <v>2.0139999999999998</v>
+        <f t="shared" si="10"/>
+        <v>2.0140000000000088E-3</v>
       </c>
       <c r="V205" s="3" t="s">
         <v>128</v>
@@ -17374,13 +17478,14 @@
         <v>128</v>
       </c>
       <c r="S206" s="3">
-        <v>33.802999999999997</v>
+        <v>3.3803E-2</v>
       </c>
       <c r="T206" s="3">
-        <v>38.25</v>
+        <v>3.8249999999999999E-2</v>
       </c>
       <c r="U206" s="3">
-        <v>4.4470000000000001</v>
+        <f t="shared" si="10"/>
+        <v>4.4469999999999996E-3</v>
       </c>
       <c r="V206" s="3" t="s">
         <v>128</v>
@@ -17451,13 +17556,14 @@
         <v>128</v>
       </c>
       <c r="S207" s="3">
-        <v>33.89</v>
+        <v>3.3890000000000003E-2</v>
       </c>
       <c r="T207" s="3">
-        <v>35.244999999999997</v>
+        <v>3.5244999999999999E-2</v>
       </c>
       <c r="U207" s="3">
-        <v>1.355</v>
+        <f t="shared" si="10"/>
+        <v>1.3549999999999951E-3</v>
       </c>
       <c r="V207" s="3" t="s">
         <v>128</v>
@@ -17528,13 +17634,14 @@
         <v>128</v>
       </c>
       <c r="S208" s="3">
-        <v>32.79</v>
+        <v>3.279E-2</v>
       </c>
       <c r="T208" s="3">
-        <v>34.369999999999997</v>
+        <v>3.4369999999999998E-2</v>
       </c>
       <c r="U208" s="3">
-        <v>1.58</v>
+        <f t="shared" si="10"/>
+        <v>1.5799999999999981E-3</v>
       </c>
       <c r="V208" s="3" t="s">
         <v>128</v>
@@ -17605,13 +17712,14 @@
         <v>128</v>
       </c>
       <c r="S209" s="3">
-        <v>34.353999999999999</v>
+        <v>3.4354000000000003E-2</v>
       </c>
       <c r="T209" s="3">
-        <v>36.476999999999997</v>
+        <v>3.6476999999999996E-2</v>
       </c>
       <c r="U209" s="3">
-        <v>2.1230000000000002</v>
+        <f t="shared" si="10"/>
+        <v>2.1229999999999929E-3</v>
       </c>
       <c r="V209" s="3" t="s">
         <v>128</v>
@@ -17682,13 +17790,14 @@
         <v>128</v>
       </c>
       <c r="S210" s="3">
-        <v>33.74</v>
+        <v>3.3739999999999999E-2</v>
       </c>
       <c r="T210" s="3">
-        <v>34.441000000000003</v>
+        <v>3.4440999999999999E-2</v>
       </c>
       <c r="U210" s="3">
-        <v>0.70099999999999996</v>
+        <f t="shared" si="10"/>
+        <v>7.0100000000000023E-4</v>
       </c>
       <c r="V210" s="3" t="s">
         <v>128</v>
@@ -17759,13 +17868,14 @@
         <v>128</v>
       </c>
       <c r="S211" s="3">
-        <v>33.950000000000003</v>
+        <v>3.3950000000000001E-2</v>
       </c>
       <c r="T211" s="3">
-        <v>35.334000000000003</v>
+        <v>3.5334000000000004E-2</v>
       </c>
       <c r="U211" s="3">
-        <v>1.3839999999999999</v>
+        <f t="shared" si="10"/>
+        <v>1.3840000000000033E-3</v>
       </c>
       <c r="V211" s="3" t="s">
         <v>128</v>
@@ -17836,13 +17946,14 @@
         <v>128</v>
       </c>
       <c r="S212" s="3">
-        <v>33.173999999999999</v>
+        <v>3.3174000000000002E-2</v>
       </c>
       <c r="T212" s="3">
-        <v>36.951000000000001</v>
+        <v>3.6950999999999998E-2</v>
       </c>
       <c r="U212" s="3">
-        <v>3.7770000000000001</v>
+        <f t="shared" si="10"/>
+        <v>3.7769999999999956E-3</v>
       </c>
       <c r="V212" s="3" t="s">
         <v>128</v>
@@ -17913,13 +18024,14 @@
         <v>128</v>
       </c>
       <c r="S213" s="3">
-        <v>34.292999999999999</v>
+        <v>3.4292999999999997E-2</v>
       </c>
       <c r="T213" s="3">
-        <v>36.082999999999998</v>
+        <v>3.6082999999999997E-2</v>
       </c>
       <c r="U213" s="3">
-        <v>1.79</v>
+        <f t="shared" si="10"/>
+        <v>1.7899999999999999E-3</v>
       </c>
       <c r="V213" s="3" t="s">
         <v>128</v>
@@ -17990,13 +18102,14 @@
         <v>128</v>
       </c>
       <c r="S214" s="3">
-        <v>32.848999999999997</v>
+        <v>3.2848999999999996E-2</v>
       </c>
       <c r="T214" s="3">
-        <v>34.743000000000002</v>
+        <v>3.4743000000000003E-2</v>
       </c>
       <c r="U214" s="3">
-        <v>1.8939999999999999</v>
+        <f t="shared" si="10"/>
+        <v>1.8940000000000068E-3</v>
       </c>
       <c r="V214" s="3" t="s">
         <v>128</v>
@@ -18067,13 +18180,14 @@
         <v>128</v>
       </c>
       <c r="S215" s="3">
-        <v>33.642000000000003</v>
+        <v>3.3642000000000005E-2</v>
       </c>
       <c r="T215" s="3">
-        <v>45.54</v>
+        <v>4.5539999999999997E-2</v>
       </c>
       <c r="U215" s="3">
-        <v>11.898</v>
+        <f t="shared" si="10"/>
+        <v>1.1897999999999992E-2</v>
       </c>
       <c r="V215" s="3" t="s">
         <v>128</v>
@@ -18144,13 +18258,14 @@
         <v>128</v>
       </c>
       <c r="S216" s="3">
-        <v>33.222999999999999</v>
+        <v>3.3222999999999996E-2</v>
       </c>
       <c r="T216" s="3">
-        <v>37.33</v>
+        <v>3.7329999999999995E-2</v>
       </c>
       <c r="U216" s="3">
-        <v>4.1070000000000002</v>
+        <f t="shared" si="10"/>
+        <v>4.1069999999999995E-3</v>
       </c>
       <c r="V216" s="3" t="s">
         <v>128</v>
@@ -18221,13 +18336,14 @@
         <v>128</v>
       </c>
       <c r="S217" s="3">
-        <v>32.970999999999997</v>
+        <v>3.2970999999999993E-2</v>
       </c>
       <c r="T217" s="3">
-        <v>34.012999999999998</v>
+        <v>3.4013000000000002E-2</v>
       </c>
       <c r="U217" s="3">
-        <v>1.042</v>
+        <f t="shared" si="10"/>
+        <v>1.0420000000000082E-3</v>
       </c>
       <c r="V217" s="3" t="s">
         <v>128</v>
@@ -18298,13 +18414,14 @@
         <v>128</v>
       </c>
       <c r="S218" s="3">
-        <v>33.847000000000001</v>
+        <v>3.3847000000000002E-2</v>
       </c>
       <c r="T218" s="3">
-        <v>34.975000000000001</v>
+        <v>3.4974999999999999E-2</v>
       </c>
       <c r="U218" s="3">
-        <v>1.1279999999999999</v>
+        <f t="shared" si="10"/>
+        <v>1.1279999999999971E-3</v>
       </c>
       <c r="V218" s="3" t="s">
         <v>128</v>
@@ -18375,13 +18492,14 @@
         <v>128</v>
       </c>
       <c r="S219" s="3">
-        <v>33.412999999999997</v>
+        <v>3.3412999999999998E-2</v>
       </c>
       <c r="T219" s="3">
-        <v>41.3</v>
+        <v>4.1299999999999996E-2</v>
       </c>
       <c r="U219" s="3">
-        <v>7.8869999999999996</v>
+        <f t="shared" si="10"/>
+        <v>7.8869999999999982E-3</v>
       </c>
       <c r="V219" s="3" t="s">
         <v>128</v>
@@ -18452,13 +18570,14 @@
         <v>128</v>
       </c>
       <c r="S220" s="3">
-        <v>32.569000000000003</v>
+        <v>3.2569000000000001E-2</v>
       </c>
       <c r="T220" s="3">
-        <v>34.701999999999998</v>
+        <v>3.4701999999999997E-2</v>
       </c>
       <c r="U220" s="3">
-        <v>2.133</v>
+        <f t="shared" si="10"/>
+        <v>2.132999999999996E-3</v>
       </c>
       <c r="V220" s="3" t="s">
         <v>128</v>
@@ -18529,13 +18648,14 @@
         <v>128</v>
       </c>
       <c r="S221" s="3">
-        <v>33.987000000000002</v>
+        <v>3.3987000000000003E-2</v>
       </c>
       <c r="T221" s="3">
-        <v>45.968000000000004</v>
+        <v>4.5968000000000002E-2</v>
       </c>
       <c r="U221" s="3">
-        <v>11.981</v>
+        <f t="shared" si="10"/>
+        <v>1.1980999999999999E-2</v>
       </c>
       <c r="V221" s="3" t="s">
         <v>128</v>
@@ -18606,13 +18726,14 @@
         <v>128</v>
       </c>
       <c r="S222" s="3">
-        <v>33.093000000000004</v>
+        <v>3.3093000000000004E-2</v>
       </c>
       <c r="T222" s="3">
-        <v>33.819000000000003</v>
+        <v>3.3819000000000002E-2</v>
       </c>
       <c r="U222" s="3">
-        <v>0.72599999999999998</v>
+        <f t="shared" si="10"/>
+        <v>7.2599999999999748E-4</v>
       </c>
       <c r="V222" s="3" t="s">
         <v>128</v>
@@ -18683,13 +18804,14 @@
         <v>128</v>
       </c>
       <c r="S223" s="3">
-        <v>33.680999999999997</v>
+        <v>3.3680999999999996E-2</v>
       </c>
       <c r="T223" s="3">
-        <v>38.442999999999998</v>
+        <v>3.8442999999999998E-2</v>
       </c>
       <c r="U223" s="3">
-        <v>4.7619999999999996</v>
+        <f t="shared" si="10"/>
+        <v>4.7620000000000023E-3</v>
       </c>
       <c r="V223" s="3" t="s">
         <v>128</v>
@@ -18760,13 +18882,14 @@
         <v>128</v>
       </c>
       <c r="S224" s="3">
-        <v>33.384</v>
+        <v>3.3383999999999997E-2</v>
       </c>
       <c r="T224" s="3">
-        <v>38.185000000000002</v>
+        <v>3.8185000000000004E-2</v>
       </c>
       <c r="U224" s="3">
-        <v>4.8010000000000002</v>
+        <f t="shared" si="10"/>
+        <v>4.8010000000000067E-3</v>
       </c>
       <c r="V224" s="3" t="s">
         <v>128</v>
@@ -18837,13 +18960,14 @@
         <v>128</v>
       </c>
       <c r="S225" s="3">
-        <v>33.497</v>
+        <v>3.3496999999999999E-2</v>
       </c>
       <c r="T225" s="3">
-        <v>34.715000000000003</v>
+        <v>3.4715000000000003E-2</v>
       </c>
       <c r="U225" s="3">
-        <v>1.218</v>
+        <f t="shared" si="10"/>
+        <v>1.2180000000000038E-3</v>
       </c>
       <c r="V225" s="3" t="s">
         <v>128</v>
@@ -18914,13 +19038,14 @@
         <v>128</v>
       </c>
       <c r="S226" s="3">
-        <v>32.401000000000003</v>
+        <v>3.2401000000000006E-2</v>
       </c>
       <c r="T226" s="3">
-        <v>33.972999999999999</v>
+        <v>3.3972999999999996E-2</v>
       </c>
       <c r="U226" s="3">
-        <v>1.5720000000000001</v>
+        <f t="shared" si="10"/>
+        <v>1.5719999999999901E-3</v>
       </c>
       <c r="V226" s="3" t="s">
         <v>128</v>
@@ -18991,13 +19116,14 @@
         <v>128</v>
       </c>
       <c r="S227" s="3">
-        <v>33.844999999999999</v>
+        <v>3.3845E-2</v>
       </c>
       <c r="T227" s="3">
-        <v>40.665999999999997</v>
+        <v>4.0665999999999994E-2</v>
       </c>
       <c r="U227" s="3">
-        <v>6.8209999999999997</v>
+        <f t="shared" si="10"/>
+        <v>6.8209999999999937E-3</v>
       </c>
       <c r="V227" s="3" t="s">
         <v>128</v>
@@ -19068,13 +19194,14 @@
         <v>128</v>
       </c>
       <c r="S228" s="3">
-        <v>34.941000000000003</v>
+        <v>3.4941E-2</v>
       </c>
       <c r="T228" s="3">
-        <v>35.783000000000001</v>
+        <v>3.5783000000000002E-2</v>
       </c>
       <c r="U228" s="3">
-        <v>0.84199999999999997</v>
+        <f t="shared" si="10"/>
+        <v>8.4200000000000247E-4</v>
       </c>
       <c r="V228" s="3" t="s">
         <v>128</v>
@@ -19145,13 +19272,14 @@
         <v>128</v>
       </c>
       <c r="S229" s="3">
-        <v>33.634</v>
+        <v>3.3633999999999997E-2</v>
       </c>
       <c r="T229" s="3">
-        <v>37.351999999999997</v>
+        <v>3.7351999999999996E-2</v>
       </c>
       <c r="U229" s="3">
-        <v>3.718</v>
+        <f t="shared" si="10"/>
+        <v>3.7179999999999991E-3</v>
       </c>
       <c r="V229" s="3" t="s">
         <v>128</v>
@@ -19222,13 +19350,14 @@
         <v>128</v>
       </c>
       <c r="S230" s="3">
-        <v>33.843000000000004</v>
+        <v>3.3843000000000005E-2</v>
       </c>
       <c r="T230" s="3">
-        <v>43.790999999999997</v>
+        <v>4.3790999999999997E-2</v>
       </c>
       <c r="U230" s="3">
-        <v>9.9480000000000004</v>
+        <f t="shared" ref="U230:U261" si="11">T230-S230</f>
+        <v>9.9479999999999916E-3</v>
       </c>
       <c r="V230" s="3" t="s">
         <v>128</v>
@@ -19299,13 +19428,14 @@
         <v>128</v>
       </c>
       <c r="S231" s="3">
-        <v>33.273000000000003</v>
+        <v>3.3273000000000004E-2</v>
       </c>
       <c r="T231" s="3">
-        <v>44.369</v>
+        <v>4.4368999999999999E-2</v>
       </c>
       <c r="U231" s="3">
-        <v>11.096</v>
+        <f t="shared" si="11"/>
+        <v>1.1095999999999995E-2</v>
       </c>
       <c r="V231" s="3" t="s">
         <v>128</v>
@@ -19376,13 +19506,14 @@
         <v>128</v>
       </c>
       <c r="S232" s="3">
-        <v>33.747999999999998</v>
+        <v>3.3748E-2</v>
       </c>
       <c r="T232" s="3">
-        <v>34.716999999999999</v>
+        <v>3.4716999999999998E-2</v>
       </c>
       <c r="U232" s="3">
-        <v>0.96899999999999997</v>
+        <f t="shared" si="11"/>
+        <v>9.6899999999999764E-4</v>
       </c>
       <c r="V232" s="3" t="s">
         <v>128</v>
@@ -19453,13 +19584,14 @@
         <v>128</v>
       </c>
       <c r="S233" s="3">
-        <v>34.896999999999998</v>
+        <v>3.4896999999999997E-2</v>
       </c>
       <c r="T233" s="3">
-        <v>38.01</v>
+        <v>3.8009999999999995E-2</v>
       </c>
       <c r="U233" s="3">
-        <v>3.113</v>
+        <f t="shared" si="11"/>
+        <v>3.1129999999999977E-3</v>
       </c>
       <c r="V233" s="3" t="s">
         <v>128</v>
@@ -19530,13 +19662,14 @@
         <v>128</v>
       </c>
       <c r="S234" s="3">
-        <v>34.47</v>
+        <v>3.4470000000000001E-2</v>
       </c>
       <c r="T234" s="3">
-        <v>35.271000000000001</v>
+        <v>3.5271000000000004E-2</v>
       </c>
       <c r="U234" s="3">
-        <v>0.80100000000000005</v>
+        <f t="shared" si="11"/>
+        <v>8.010000000000031E-4</v>
       </c>
       <c r="V234" s="3" t="s">
         <v>128</v>
@@ -19607,13 +19740,14 @@
         <v>128</v>
       </c>
       <c r="S235" s="3">
-        <v>33.594999999999999</v>
+        <v>3.3595E-2</v>
       </c>
       <c r="T235" s="3">
-        <v>34.902000000000001</v>
+        <v>3.4902000000000002E-2</v>
       </c>
       <c r="U235" s="3">
-        <v>1.3069999999999999</v>
+        <f t="shared" si="11"/>
+        <v>1.3070000000000026E-3</v>
       </c>
       <c r="V235" s="3" t="s">
         <v>128</v>
@@ -19684,13 +19818,14 @@
         <v>128</v>
       </c>
       <c r="S236" s="3">
-        <v>33.136000000000003</v>
+        <v>3.3136000000000006E-2</v>
       </c>
       <c r="T236" s="3">
-        <v>35.917000000000002</v>
+        <v>3.5917000000000004E-2</v>
       </c>
       <c r="U236" s="3">
-        <v>2.7810000000000001</v>
+        <f t="shared" si="11"/>
+        <v>2.7809999999999988E-3</v>
       </c>
       <c r="V236" s="3" t="s">
         <v>128</v>
@@ -19761,13 +19896,14 @@
         <v>128</v>
       </c>
       <c r="S237" s="3">
-        <v>32.703000000000003</v>
+        <v>3.2703000000000003E-2</v>
       </c>
       <c r="T237" s="3">
-        <v>35.405000000000001</v>
+        <v>3.5404999999999999E-2</v>
       </c>
       <c r="U237" s="3">
-        <v>2.702</v>
+        <f t="shared" si="11"/>
+        <v>2.7019999999999961E-3</v>
       </c>
       <c r="V237" s="3" t="s">
         <v>128</v>
@@ -19838,13 +19974,14 @@
         <v>128</v>
       </c>
       <c r="S238" s="3">
-        <v>33.223999999999997</v>
+        <v>3.3223999999999997E-2</v>
       </c>
       <c r="T238" s="3">
-        <v>37.569000000000003</v>
+        <v>3.7569000000000005E-2</v>
       </c>
       <c r="U238" s="3">
-        <v>4.3449999999999998</v>
+        <f t="shared" si="11"/>
+        <v>4.3450000000000086E-3</v>
       </c>
       <c r="V238" s="3" t="s">
         <v>128</v>
@@ -19915,13 +20052,14 @@
         <v>128</v>
       </c>
       <c r="S239" s="3">
-        <v>33.540999999999997</v>
+        <v>3.3540999999999994E-2</v>
       </c>
       <c r="T239" s="3">
-        <v>35.284999999999997</v>
+        <v>3.5284999999999997E-2</v>
       </c>
       <c r="U239" s="3">
-        <v>1.744</v>
+        <f t="shared" si="11"/>
+        <v>1.7440000000000025E-3</v>
       </c>
       <c r="V239" s="3" t="s">
         <v>128</v>
@@ -19992,13 +20130,14 @@
         <v>128</v>
       </c>
       <c r="S240" s="3">
-        <v>33.651000000000003</v>
+        <v>3.3651E-2</v>
       </c>
       <c r="T240" s="3">
-        <v>35.090000000000003</v>
+        <v>3.5090000000000003E-2</v>
       </c>
       <c r="U240" s="3">
-        <v>1.4390000000000001</v>
+        <f t="shared" si="11"/>
+        <v>1.4390000000000028E-3</v>
       </c>
       <c r="V240" s="3" t="s">
         <v>128</v>
@@ -20069,13 +20208,14 @@
         <v>128</v>
       </c>
       <c r="S241" s="3">
-        <v>33.081000000000003</v>
+        <v>3.3081000000000006E-2</v>
       </c>
       <c r="T241" s="3">
-        <v>33.758000000000003</v>
+        <v>3.3758000000000003E-2</v>
       </c>
       <c r="U241" s="3">
-        <v>0.67700000000000005</v>
+        <f t="shared" si="11"/>
+        <v>6.7699999999999705E-4</v>
       </c>
       <c r="V241" s="3" t="s">
         <v>128</v>
@@ -20146,13 +20286,14 @@
         <v>128</v>
       </c>
       <c r="S242" s="3">
-        <v>33.057000000000002</v>
+        <v>3.3057000000000003E-2</v>
       </c>
       <c r="T242" s="3">
-        <v>34.170999999999999</v>
+        <v>3.4171E-2</v>
       </c>
       <c r="U242" s="3">
-        <v>1.1140000000000001</v>
+        <f t="shared" si="11"/>
+        <v>1.1139999999999969E-3</v>
       </c>
       <c r="V242" s="3" t="s">
         <v>128</v>
@@ -20223,13 +20364,14 @@
         <v>128</v>
       </c>
       <c r="S243" s="3">
-        <v>33.713999999999999</v>
+        <v>3.3714000000000001E-2</v>
       </c>
       <c r="T243" s="3">
-        <v>38.243000000000002</v>
+        <v>3.8242999999999999E-2</v>
       </c>
       <c r="U243" s="3">
-        <v>4.5289999999999999</v>
+        <f t="shared" si="11"/>
+        <v>4.5289999999999983E-3</v>
       </c>
       <c r="V243" s="3" t="s">
         <v>128</v>
@@ -20300,13 +20442,14 @@
         <v>128</v>
       </c>
       <c r="S244" s="3">
-        <v>33.630000000000003</v>
+        <v>3.363E-2</v>
       </c>
       <c r="T244" s="3">
-        <v>33.893000000000001</v>
+        <v>3.3893E-2</v>
       </c>
       <c r="U244" s="3">
-        <v>0.26300000000000001</v>
+        <f t="shared" si="11"/>
+        <v>2.6299999999999935E-4</v>
       </c>
       <c r="V244" s="3" t="s">
         <v>128</v>
@@ -20377,13 +20520,14 @@
         <v>128</v>
       </c>
       <c r="S245" s="3">
-        <v>33.335999999999999</v>
+        <v>3.3335999999999998E-2</v>
       </c>
       <c r="T245" s="3">
-        <v>33.752000000000002</v>
+        <v>3.3752000000000004E-2</v>
       </c>
       <c r="U245" s="3">
-        <v>0.41599999999999998</v>
+        <f t="shared" si="11"/>
+        <v>4.1600000000000664E-4</v>
       </c>
       <c r="V245" s="3" t="s">
         <v>128</v>
@@ -20454,13 +20598,14 @@
         <v>128</v>
       </c>
       <c r="S246" s="3">
-        <v>33.637</v>
+        <v>3.3637E-2</v>
       </c>
       <c r="T246" s="3">
-        <v>35.874000000000002</v>
+        <v>3.5874000000000003E-2</v>
       </c>
       <c r="U246" s="3">
-        <v>2.2370000000000001</v>
+        <f t="shared" si="11"/>
+        <v>2.2370000000000029E-3</v>
       </c>
       <c r="V246" s="3" t="s">
         <v>128</v>
@@ -20531,13 +20676,14 @@
         <v>128</v>
       </c>
       <c r="S247" s="3">
-        <v>34.070999999999998</v>
+        <v>3.4070999999999997E-2</v>
       </c>
       <c r="T247" s="3">
-        <v>37.493000000000002</v>
+        <v>3.7493000000000005E-2</v>
       </c>
       <c r="U247" s="3">
-        <v>3.4220000000000002</v>
+        <f t="shared" si="11"/>
+        <v>3.4220000000000084E-3</v>
       </c>
       <c r="V247" s="3" t="s">
         <v>128</v>
@@ -20608,13 +20754,14 @@
         <v>128</v>
       </c>
       <c r="S248" s="3">
-        <v>33.994</v>
+        <v>3.3993999999999996E-2</v>
       </c>
       <c r="T248" s="3">
-        <v>36.134</v>
+        <v>3.6133999999999999E-2</v>
       </c>
       <c r="U248" s="3">
-        <v>2.14</v>
+        <f t="shared" si="11"/>
+        <v>2.140000000000003E-3</v>
       </c>
       <c r="V248" s="3" t="s">
         <v>128</v>
@@ -20685,13 +20832,14 @@
         <v>128</v>
       </c>
       <c r="S249" s="3">
-        <v>33.734999999999999</v>
+        <v>3.3735000000000001E-2</v>
       </c>
       <c r="T249" s="3">
-        <v>36.25</v>
+        <v>3.6249999999999998E-2</v>
       </c>
       <c r="U249" s="3">
-        <v>2.5150000000000001</v>
+        <f t="shared" si="11"/>
+        <v>2.5149999999999964E-3</v>
       </c>
       <c r="V249" s="3" t="s">
         <v>128</v>
@@ -20762,13 +20910,14 @@
         <v>128</v>
       </c>
       <c r="S250" s="3">
-        <v>33.561999999999998</v>
+        <v>3.3561999999999995E-2</v>
       </c>
       <c r="T250" s="3">
-        <v>35.939</v>
+        <v>3.5938999999999999E-2</v>
       </c>
       <c r="U250" s="3">
-        <v>2.3769999999999998</v>
+        <f t="shared" si="11"/>
+        <v>2.3770000000000041E-3</v>
       </c>
       <c r="V250" s="3" t="s">
         <v>128</v>
@@ -20839,13 +20988,14 @@
         <v>128</v>
       </c>
       <c r="S251" s="3">
-        <v>33.133000000000003</v>
+        <v>3.3133000000000003E-2</v>
       </c>
       <c r="T251" s="3">
-        <v>33.755000000000003</v>
+        <v>3.3755E-2</v>
       </c>
       <c r="U251" s="3">
-        <v>0.622</v>
+        <f t="shared" si="11"/>
+        <v>6.2199999999999755E-4</v>
       </c>
       <c r="V251" s="3" t="s">
         <v>128</v>
@@ -20916,13 +21066,14 @@
         <v>128</v>
       </c>
       <c r="S252" s="3">
-        <v>33.225999999999999</v>
+        <v>3.3225999999999999E-2</v>
       </c>
       <c r="T252" s="3">
-        <v>38.152999999999999</v>
+        <v>3.8152999999999999E-2</v>
       </c>
       <c r="U252" s="3">
-        <v>4.9269999999999996</v>
+        <f t="shared" si="11"/>
+        <v>4.9270000000000008E-3</v>
       </c>
       <c r="V252" s="3" t="s">
         <v>128</v>
@@ -20993,13 +21144,14 @@
         <v>128</v>
       </c>
       <c r="S253" s="3">
-        <v>33.817</v>
+        <v>3.3817E-2</v>
       </c>
       <c r="T253" s="3">
-        <v>36.069000000000003</v>
+        <v>3.6069000000000004E-2</v>
       </c>
       <c r="U253" s="3">
-        <v>2.2519999999999998</v>
+        <f t="shared" si="11"/>
+        <v>2.252000000000004E-3</v>
       </c>
       <c r="V253" s="3" t="s">
         <v>128</v>
@@ -21070,13 +21222,14 @@
         <v>128</v>
       </c>
       <c r="S254" s="3">
-        <v>33.968000000000004</v>
+        <v>3.3968000000000005E-2</v>
       </c>
       <c r="T254" s="3">
-        <v>38.051000000000002</v>
+        <v>3.8051000000000001E-2</v>
       </c>
       <c r="U254" s="3">
-        <v>4.0830000000000002</v>
+        <f t="shared" si="11"/>
+        <v>4.0829999999999964E-3</v>
       </c>
       <c r="V254" s="3" t="s">
         <v>128</v>
@@ -21147,13 +21300,14 @@
         <v>128</v>
       </c>
       <c r="S255" s="3">
-        <v>33.621000000000002</v>
+        <v>3.3621000000000005E-2</v>
       </c>
       <c r="T255" s="3">
-        <v>34.505000000000003</v>
+        <v>3.4505000000000001E-2</v>
       </c>
       <c r="U255" s="3">
-        <v>0.88400000000000001</v>
+        <f t="shared" si="11"/>
+        <v>8.839999999999959E-4</v>
       </c>
       <c r="V255" s="3" t="s">
         <v>128</v>
@@ -21224,13 +21378,14 @@
         <v>128</v>
       </c>
       <c r="S256" s="3">
-        <v>33.408999999999999</v>
+        <v>3.3409000000000001E-2</v>
       </c>
       <c r="T256" s="3">
-        <v>35.067</v>
+        <v>3.5067000000000001E-2</v>
       </c>
       <c r="U256" s="3">
-        <v>1.6579999999999999</v>
+        <f t="shared" si="11"/>
+        <v>1.6579999999999998E-3</v>
       </c>
       <c r="V256" s="3" t="s">
         <v>128</v>
@@ -21301,13 +21456,14 @@
         <v>128</v>
       </c>
       <c r="S257" s="3">
-        <v>34.479999999999997</v>
+        <v>3.4479999999999997E-2</v>
       </c>
       <c r="T257" s="3">
-        <v>37.274999999999999</v>
+        <v>3.7274999999999996E-2</v>
       </c>
       <c r="U257" s="3">
-        <v>2.7949999999999999</v>
+        <f t="shared" si="11"/>
+        <v>2.7949999999999989E-3</v>
       </c>
       <c r="V257" s="3" t="s">
         <v>128</v>
@@ -21378,13 +21534,14 @@
         <v>128</v>
       </c>
       <c r="S258" s="3">
-        <v>33.6</v>
+        <v>3.3600000000000005E-2</v>
       </c>
       <c r="T258" s="3">
-        <v>40.649000000000001</v>
+        <v>4.0648999999999998E-2</v>
       </c>
       <c r="U258" s="3">
-        <v>7.0490000000000004</v>
+        <f t="shared" si="11"/>
+        <v>7.0489999999999928E-3</v>
       </c>
       <c r="V258" s="3" t="s">
         <v>128</v>
@@ -21455,13 +21612,14 @@
         <v>128</v>
       </c>
       <c r="S259" s="3">
-        <v>33.408000000000001</v>
+        <v>3.3408E-2</v>
       </c>
       <c r="T259" s="3">
-        <v>34.002000000000002</v>
+        <v>3.4002000000000004E-2</v>
       </c>
       <c r="U259" s="3">
-        <v>0.59399999999999997</v>
+        <f t="shared" si="11"/>
+        <v>5.9400000000000425E-4</v>
       </c>
       <c r="V259" s="3" t="s">
         <v>128</v>
@@ -21532,13 +21690,14 @@
         <v>128</v>
       </c>
       <c r="S260" s="3">
-        <v>33.366999999999997</v>
+        <v>3.3366999999999994E-2</v>
       </c>
       <c r="T260" s="3">
-        <v>37.865000000000002</v>
+        <v>3.7865000000000003E-2</v>
       </c>
       <c r="U260" s="3">
-        <v>4.4980000000000002</v>
+        <f t="shared" si="11"/>
+        <v>4.4980000000000089E-3</v>
       </c>
       <c r="V260" s="3" t="s">
         <v>128</v>
@@ -21609,13 +21768,14 @@
         <v>128</v>
       </c>
       <c r="S261" s="3">
-        <v>33.792999999999999</v>
+        <v>3.3792999999999997E-2</v>
       </c>
       <c r="T261" s="3">
-        <v>38.048000000000002</v>
+        <v>3.8047999999999998E-2</v>
       </c>
       <c r="U261" s="3">
-        <v>4.2549999999999999</v>
+        <f t="shared" si="11"/>
+        <v>4.2550000000000018E-3</v>
       </c>
       <c r="V261" s="3" t="s">
         <v>128</v>

</xml_diff>